<commit_message>
Changed file structure, Finished Implementation and Evaluation Chapters, reagganged test files for Application and Design
</commit_message>
<xml_diff>
--- a/Documents/Sprint Planning/AFNT Progress Calculator.xlsx
+++ b/Documents/Sprint Planning/AFNT Progress Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/Sprint Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{1879444F-A13A-42C2-B723-32323209AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F76ED91-EF03-4967-953B-CB33C2B6E625}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{1879444F-A13A-42C2-B723-32323209AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A657CA1-E434-45F2-8203-80A3B5C120EE}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3630" windowWidth="19200" windowHeight="21150" xr2:uid="{222EAB01-4AFD-487B-935F-D69428DA4116}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{222EAB01-4AFD-487B-935F-D69428DA4116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>Partically Complete</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Total Requirements</t>
   </si>
   <si>
-    <t>Total Partically Completed</t>
-  </si>
-  <si>
     <t>Total Not Implementing</t>
   </si>
   <si>
@@ -114,6 +108,12 @@
   </si>
   <si>
     <t>Percentage Completed</t>
+  </si>
+  <si>
+    <t>Partially Complete</t>
+  </si>
+  <si>
+    <t>Total Partially Completed</t>
   </si>
 </sst>
 </file>
@@ -220,6 +220,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,7 +546,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A11" sqref="A11:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,19 +564,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -598,7 +602,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>7</v>
@@ -619,7 +623,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -640,7 +644,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -661,7 +665,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -674,27 +678,27 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -715,7 +719,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -736,7 +740,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -757,7 +761,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -778,7 +782,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -799,7 +803,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -820,7 +824,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -841,7 +845,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -862,7 +866,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -883,7 +887,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -896,7 +900,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3">
         <f>SUM(D6,D18)</f>
@@ -906,7 +910,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3">
         <f>SUM(B2:B5,B9:B17)</f>
@@ -916,7 +920,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <f>SUM(C2:C5,C9:C17)</f>
@@ -928,7 +932,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3">
         <f>SUM(D2:D5,D9:D17)</f>
@@ -940,7 +944,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
         <f>SUM(E2:E5,E9:E17)</f>
@@ -952,7 +956,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3">
         <f>B20-B21</f>
@@ -961,7 +965,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="4">
         <f>ROUNDUP(((C24*B24) + (C23*B23) + (B22*C22))/B26*100, 0)</f>

</xml_diff>